<commit_message>
Fixed capital letter error
</commit_message>
<xml_diff>
--- a/small_data.xlsx
+++ b/small_data.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Иванов Михаил Сергеевич</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>Диплом 2 степени</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>дательный</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +456,7 @@
     <col min="5" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -482,8 +488,11 @@
       <c r="M1" t="s">
         <v>21</v>
       </c>
+      <c r="N1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -514,8 +523,11 @@
       <c r="M2" t="s">
         <v>22</v>
       </c>
+      <c r="N2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -547,7 +559,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>

</xml_diff>